<commit_message>
Deploying to gh-pages from @ eurovibes/huibike@27b0568947115e0d296c15c50f3c558930dfdfed 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/huibike-bom_0.1.xlsx
+++ b/Fabrication/BoM/huibike-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Row</t>
   </si>
@@ -53,19 +53,154 @@
     <t/>
   </si>
   <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>CL05B104KO5NNNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>C1525</t>
+  </si>
+  <si>
+    <t>C_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>16V 100nF X7R ±10% 0402  Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>1 µF</t>
   </si>
   <si>
-    <t>C28323 C1525 C8056 C475630 C25756 C128438 C58069</t>
+    <t>CL21B105KBFNNNE</t>
+  </si>
+  <si>
+    <t>C28323</t>
   </si>
   <si>
     <t>C_0805_2012Metric</t>
   </si>
   <si>
-    <t>Unpolarized capacitor</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>50V 1uF X7R ±10% 0805 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>ZMM3V3-M</t>
+  </si>
+  <si>
+    <t>ST(Semtech)</t>
+  </si>
+  <si>
+    <t>C8056</t>
+  </si>
+  <si>
+    <t>D_MiniMELF</t>
+  </si>
+  <si>
+    <t>Single 3.1V~3.5V 500mW 3.3V LL-34 Zener Diodes ROHS</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>PinHeader_1x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>BC847</t>
+  </si>
+  <si>
+    <t>Shikues</t>
+  </si>
+  <si>
+    <t>C475630</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>45V 200mW 100mA NPN SOT-23 Bipolar Transistors - BJT ROHS</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>15 kΩ</t>
+  </si>
+  <si>
+    <t>0402WGF1502TCE</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
+    <t>C25756</t>
+  </si>
+  <si>
+    <t>R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>62.5mW Thick Film Resistors ±1% 15kΩ 0402 Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>ATtiny10-TS</t>
+  </si>
+  <si>
+    <t>ATTINY10-TSHR</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>C128438</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>AVR 32Byte 12MHz 4 SOT-23-6 Microcontroller Units (MCUs/MPUs/SOCs) ROHS</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>LM78M05_TO252</t>
+  </si>
+  <si>
+    <t>L78M05ABDT-TR</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>C58069</t>
+  </si>
+  <si>
+    <t>TO-252-2</t>
+  </si>
+  <si>
+    <t>2dB@(120Hz) 500mA Fixed 5V~5V Positive 35V TO-252-2(DPAK) Linear Voltage Regulators (LDO) ROHS</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -161,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +327,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0FFF4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF0BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -205,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -228,6 +381,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,8 +410,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>182573</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:colOff>582623</xdr:colOff>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>1598</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -574,7 +736,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -585,18 +747,18 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="60.7109375" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -607,27 +769,27 @@
     </row>
     <row r="2" spans="1:9">
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="F3" s="3">
         <v>17</v>
@@ -635,13 +797,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="F4" s="3">
         <v>17</v>
@@ -649,13 +811,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -663,13 +825,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="F6" s="3">
         <v>17</v>
@@ -704,7 +866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -715,22 +877,225 @@
         <v>11</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>15</v>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -756,17 +1121,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>